<commit_message>
11 testcases on Multi Reshcdule
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4650-DISB01JAN2015-RESCHDULE01FEB2015-INSTRESCHDULE15FEB2015.xlsx
+++ b/Mifos Automation Excels/Client/4650-DISB01JAN2015-RESCHDULE01FEB2015-INSTRESCHDULE15FEB2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="1" r:id="rId1"/>
@@ -630,7 +630,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,8 +859,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,13 +955,13 @@
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
       <c r="F3" s="9">
-        <v>738.49</v>
+        <v>788.49</v>
       </c>
       <c r="G3" s="12">
-        <v>9261.51</v>
+        <v>9211.51</v>
       </c>
       <c r="H3" s="9">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="I3" s="9">
         <v>0</v>
@@ -999,13 +999,13 @@
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9">
-        <v>795.87</v>
+        <v>796.37</v>
       </c>
       <c r="G4" s="12">
-        <v>8465.64</v>
+        <v>8415.14</v>
       </c>
       <c r="H4" s="9">
-        <v>92.62</v>
+        <v>92.12</v>
       </c>
       <c r="I4" s="9">
         <v>0</v>
@@ -1043,13 +1043,13 @@
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9">
-        <v>803.83</v>
+        <v>804.34</v>
       </c>
       <c r="G5" s="12">
-        <v>7661.81</v>
+        <v>7610.8</v>
       </c>
       <c r="H5" s="9">
-        <v>84.66</v>
+        <v>84.15</v>
       </c>
       <c r="I5" s="9">
         <v>0</v>
@@ -1087,13 +1087,13 @@
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9">
-        <v>811.87</v>
+        <v>812.38</v>
       </c>
       <c r="G6" s="12">
-        <v>6849.94</v>
+        <v>6798.42</v>
       </c>
       <c r="H6" s="9">
-        <v>76.62</v>
+        <v>76.11</v>
       </c>
       <c r="I6" s="9">
         <v>0</v>
@@ -1131,13 +1131,13 @@
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9">
-        <v>819.99</v>
+        <v>820.51</v>
       </c>
       <c r="G7" s="12">
-        <v>6029.95</v>
+        <v>5977.91</v>
       </c>
       <c r="H7" s="9">
-        <v>68.5</v>
+        <v>67.98</v>
       </c>
       <c r="I7" s="9">
         <v>0</v>
@@ -1175,13 +1175,13 @@
       <c r="D8" s="9"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9">
-        <v>828.19</v>
+        <v>828.71</v>
       </c>
       <c r="G8" s="12">
-        <v>5201.76</v>
+        <v>5149.2</v>
       </c>
       <c r="H8" s="9">
-        <v>60.3</v>
+        <v>59.78</v>
       </c>
       <c r="I8" s="9">
         <v>0</v>
@@ -1219,13 +1219,13 @@
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9">
-        <v>836.47</v>
+        <v>837</v>
       </c>
       <c r="G9" s="12">
-        <v>4365.29</v>
+        <v>4312.2</v>
       </c>
       <c r="H9" s="9">
-        <v>52.02</v>
+        <v>51.49</v>
       </c>
       <c r="I9" s="9">
         <v>0</v>
@@ -1263,13 +1263,13 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9">
-        <v>844.84</v>
+        <v>845.37</v>
       </c>
       <c r="G10" s="12">
-        <v>3520.45</v>
+        <v>3466.83</v>
       </c>
       <c r="H10" s="9">
-        <v>43.65</v>
+        <v>43.12</v>
       </c>
       <c r="I10" s="9">
         <v>0</v>
@@ -1307,13 +1307,13 @@
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9">
-        <v>853.29</v>
+        <v>853.82</v>
       </c>
       <c r="G11" s="12">
-        <v>2667.16</v>
+        <v>2613.0100000000002</v>
       </c>
       <c r="H11" s="9">
-        <v>35.200000000000003</v>
+        <v>34.67</v>
       </c>
       <c r="I11" s="9">
         <v>0</v>
@@ -1351,13 +1351,13 @@
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9">
-        <v>861.82</v>
+        <v>862.36</v>
       </c>
       <c r="G12" s="12">
-        <v>1805.34</v>
+        <v>1750.65</v>
       </c>
       <c r="H12" s="9">
-        <v>26.67</v>
+        <v>26.13</v>
       </c>
       <c r="I12" s="9">
         <v>0</v>
@@ -1395,13 +1395,13 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9">
-        <v>870.44</v>
+        <v>870.98</v>
       </c>
       <c r="G13" s="9">
-        <v>934.9</v>
+        <v>879.67</v>
       </c>
       <c r="H13" s="9">
-        <v>18.05</v>
+        <v>17.510000000000002</v>
       </c>
       <c r="I13" s="9">
         <v>0</v>
@@ -1439,13 +1439,13 @@
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9">
-        <v>934.9</v>
+        <v>879.67</v>
       </c>
       <c r="G14" s="9">
         <v>0</v>
       </c>
       <c r="H14" s="9">
-        <v>9.35</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="I14" s="9">
         <v>0</v>
@@ -1454,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="9">
-        <v>944.25</v>
+        <v>888.47</v>
       </c>
       <c r="L14" s="9">
         <v>0</v>
@@ -1467,7 +1467,7 @@
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="9">
-        <v>944.25</v>
+        <v>888.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>